<commit_message>
màj tableau de synthèse
</commit_message>
<xml_diff>
--- a/public/competence/Tableau de synthèse SLAM - Epreuve E4 - BTS SIO 2025.xlsx
+++ b/public/competence/Tableau de synthèse SLAM - Epreuve E4 - BTS SIO 2025.xlsx
@@ -8,22 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxime/Desktop/portoflio/public/competence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0CC0004-AFB3-A24C-842D-DBF0931D367C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F241671E-39DB-424B-AC56-220FE300FF52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tableau de synthèse Épreuve E4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Tableau de synthèse Épreuve E4'!$A$1:$H$18</definedName>
   </definedNames>
   <calcPr calcId="101716"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Gérer le patrimoine informatique</t>
   </si>
@@ -133,36 +133,9 @@
     <t>SESSION 2025</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>15-05-2024 au 28/06/2024</t>
   </si>
   <si>
-    <t>Déploiement et intégrement du site web, interface homme-machine, affichage des donnnées des capteurs de l'entreprise</t>
-  </si>
-  <si>
-    <t>Gestion d'utilisateurs, login, rôles, droits, sécurité des connexions (JWT, etc), stockage dans des cookies</t>
-  </si>
-  <si>
-    <t>Gestion des sauvegardes de la machine virtuelle Kuzzle et des données Kuzzle</t>
-  </si>
-  <si>
-    <t>Développement du site en accord avec un cahier des charges de l'entreprise (fonctionnalités demandées, charte graphique, …)</t>
-  </si>
-  <si>
-    <t>Auto Formation sur Kuzzle, Vue.js, TypeScript et les plugins implémentés (Chart.js, NodeMailer) pour arriver aux objectifs fixés</t>
-  </si>
-  <si>
-    <t>Projection sur les fonctionnalités à implémenter en dehors du cahier des charges donnés par l'entreprise</t>
-  </si>
-  <si>
-    <t>Utilisation d'une machine virtuelle Debian 12 (du terminal) pour accèder aux codes de l'application web</t>
-  </si>
-  <si>
-    <t>Gestion des trames HTTPS de capteurs, décodeurs, traiter les données de ces trames dans le backend, les stocker et les afficher dans le frontend</t>
-  </si>
-  <si>
     <t>NOM et prénom : Brunin Maxime</t>
   </si>
   <si>
@@ -170,6 +143,30 @@
   </si>
   <si>
     <t>Adresse URL du portfolio : maximebrunin.vercel.app</t>
+  </si>
+  <si>
+    <t>Développement Marieteam web et logiciel</t>
+  </si>
+  <si>
+    <t>Installer un serveur GLPI, gérer les habilitations, mettre en place un collecteur, mettre en place un HAProxy</t>
+  </si>
+  <si>
+    <t>Veille Technologique sur les moteurs de jeu vidéos</t>
+  </si>
+  <si>
+    <t>Développemnt du portfolio en Next.js</t>
+  </si>
+  <si>
+    <t>Développement d'un site en IOT pour la gestion de données des capteurs en Vue.js, Kuzzle</t>
+  </si>
+  <si>
+    <t>Développement d'une application mobile sous Android Studio en Kotlin, relié à une API REST et une base de données</t>
+  </si>
+  <si>
+    <t>24-02-2025 au 04-04-2025</t>
+  </si>
+  <si>
+    <t>Autoformation sur Unity pour mon projet professionnel</t>
   </si>
 </sst>
 </file>
@@ -255,15 +252,21 @@
       <charset val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="32">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -368,51 +371,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </left>
-      <right style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </right>
-      <top style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
-      </top>
-      <bottom style="medium">
-        <color theme="2" tint="-0.749992370372631"/>
-      </bottom>
-      <diagonal/>
-    </border>
     <border diagonalDown="1">
       <left style="medium">
         <color theme="2" tint="-0.749992370372631"/>
@@ -650,38 +608,59 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
       <right style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </right>
       <top style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </top>
-      <bottom style="thin">
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </left>
       <right style="thin">
         <color theme="2" tint="-0.749992370372631"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color theme="2" tint="-0.749992370372631"/>
+      <top style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
+      <left style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </left>
+      <right style="medium">
         <color theme="2" tint="-0.749992370372631"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="thin">
+        <color theme="2" tint="-0.749992370372631"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -717,14 +696,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -732,45 +705,54 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -780,56 +762,53 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1141,8 +1120,8 @@
   </sheetPr>
   <dimension ref="A1:AQ82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:H5"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1155,83 +1134,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26" t="s">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="H1" s="26"/>
+      <c r="H1" s="17"/>
     </row>
     <row r="2" spans="1:43" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
     </row>
     <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="39" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="45" t="s">
+      <c r="A3" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="40"/>
-      <c r="H3" s="46"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="25"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="43"/>
-      <c r="C4" s="43"/>
-      <c r="D4" s="43"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="12" t="s">
+      <c r="A4" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="22"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="14" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="37"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="38"/>
+      <c r="A5" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="39"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="34" t="s">
+      <c r="B6" s="35" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1254,24 +1233,24 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="25"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="20" t="s">
+      <c r="A7" s="27"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="20" t="s">
+      <c r="D7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="20" t="s">
+      <c r="E7" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="20" t="s">
+      <c r="F7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="21" t="s">
+      <c r="H7" s="16" t="s">
         <v>14</v>
       </c>
       <c r="I7"/>
@@ -1311,16 +1290,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="28"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-      <c r="G8" s="28"/>
-      <c r="H8" s="29"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
+      <c r="G8" s="29"/>
+      <c r="H8" s="30"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1358,14 +1337,16 @@
       <c r="AQ8"/>
     </row>
     <row r="9" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="9"/>
+      <c r="A9" s="9" t="s">
+        <v>28</v>
+      </c>
       <c r="B9" s="8"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
+      <c r="C9" s="40"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="12"/>
+      <c r="H9" s="42"/>
       <c r="I9"/>
       <c r="J9"/>
       <c r="K9"/>
@@ -1403,14 +1384,16 @@
       <c r="AQ9"/>
     </row>
     <row r="10" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="9"/>
+      <c r="A10" s="9" t="s">
+        <v>29</v>
+      </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="13"/>
       <c r="I10"/>
       <c r="J10"/>
       <c r="K10"/>
@@ -1448,14 +1431,16 @@
       <c r="AQ10"/>
     </row>
     <row r="11" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="9"/>
+      <c r="A11" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="42"/>
       <c r="I11"/>
       <c r="J11"/>
       <c r="K11"/>
@@ -1493,14 +1478,16 @@
       <c r="AQ11"/>
     </row>
     <row r="12" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="9"/>
+      <c r="A12" s="9" t="s">
+        <v>31</v>
+      </c>
       <c r="B12" s="8"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
-      <c r="G12" s="15"/>
-      <c r="H12" s="16"/>
+      <c r="C12" s="12"/>
+      <c r="D12" s="12"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="42"/>
       <c r="I12"/>
       <c r="J12"/>
       <c r="K12"/>
@@ -1538,14 +1525,16 @@
       <c r="AQ12"/>
     </row>
     <row r="13" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="9"/>
+      <c r="A13" s="9" t="s">
+        <v>35</v>
+      </c>
       <c r="B13" s="8"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
-      <c r="H13" s="16"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="42"/>
       <c r="I13"/>
       <c r="J13"/>
       <c r="K13"/>
@@ -1583,14 +1572,16 @@
       <c r="AQ13"/>
     </row>
     <row r="14" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="9"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="16"/>
+      <c r="A14" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="33"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1628,14 +1619,18 @@
       <c r="AQ14"/>
     </row>
     <row r="15" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="9"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="15"/>
-      <c r="H15" s="16"/>
+      <c r="A15" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="42"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1673,14 +1668,16 @@
       <c r="AQ15"/>
     </row>
     <row r="16" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="9"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="16"/>
+      <c r="A16" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="33"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1717,15 +1714,19 @@
       <c r="AP16"/>
       <c r="AQ16"/>
     </row>
-    <row r="17" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="9"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="16"/>
+    <row r="17" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45"/>
+      <c r="E17" s="45"/>
+      <c r="F17" s="45"/>
+      <c r="G17" s="45"/>
+      <c r="H17" s="46"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1763,14 +1764,14 @@
       <c r="AQ17"/>
     </row>
     <row r="18" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="9"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="16"/>
+      <c r="A18" s="5"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1807,17 +1808,15 @@
       <c r="AP18"/>
       <c r="AQ18"/>
     </row>
-    <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A19" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="31"/>
-      <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
-      <c r="H19" s="32"/>
+    <row r="19" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -1855,22 +1854,14 @@
       <c r="AQ19"/>
     </row>
     <row r="20" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B20" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G20" s="15"/>
-      <c r="H20" s="16"/>
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
       <c r="I20"/>
       <c r="J20"/>
       <c r="K20"/>
@@ -1908,24 +1899,14 @@
       <c r="AQ20"/>
     </row>
     <row r="21" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F21" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G21" s="15"/>
-      <c r="H21" s="16"/>
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
       <c r="I21"/>
       <c r="J21"/>
       <c r="K21"/>
@@ -1963,24 +1944,14 @@
       <c r="AQ21"/>
     </row>
     <row r="22" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
       <c r="I22"/>
       <c r="J22"/>
       <c r="K22"/>
@@ -2018,20 +1989,14 @@
       <c r="AQ22"/>
     </row>
     <row r="23" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="G23" s="15"/>
-      <c r="H23" s="16"/>
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
       <c r="I23"/>
       <c r="J23"/>
       <c r="K23"/>
@@ -2069,24 +2034,14 @@
       <c r="AQ23"/>
     </row>
     <row r="24" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="15"/>
-      <c r="G24" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H24" s="16"/>
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
       <c r="I24"/>
       <c r="J24"/>
       <c r="K24"/>
@@ -2124,22 +2079,14 @@
       <c r="AQ24"/>
     </row>
     <row r="25" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H25" s="16" t="s">
-        <v>24</v>
-      </c>
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
       <c r="I25"/>
       <c r="J25"/>
       <c r="K25"/>
@@ -2177,24 +2124,14 @@
       <c r="AQ25"/>
     </row>
     <row r="26" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C26" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="H26" s="16"/>
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
       <c r="I26"/>
       <c r="J26"/>
       <c r="K26"/>
@@ -2232,24 +2169,14 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="16"/>
+      <c r="A27"/>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2286,17 +2213,15 @@
       <c r="AP27"/>
       <c r="AQ27"/>
     </row>
-    <row r="28" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="A28" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="31"/>
-      <c r="F28" s="31"/>
-      <c r="G28" s="31"/>
-      <c r="H28" s="32"/>
+    <row r="28" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A28"/>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
       <c r="I28"/>
       <c r="J28"/>
       <c r="K28"/>
@@ -2334,14 +2259,14 @@
       <c r="AQ28"/>
     </row>
     <row r="29" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="9"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="16"/>
+      <c r="A29"/>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
       <c r="I29"/>
       <c r="J29"/>
       <c r="K29"/>
@@ -2379,14 +2304,14 @@
       <c r="AQ29"/>
     </row>
     <row r="30" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="9"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="16"/>
+      <c r="A30"/>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
       <c r="I30"/>
       <c r="J30"/>
       <c r="K30"/>
@@ -2424,14 +2349,14 @@
       <c r="AQ30"/>
     </row>
     <row r="31" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="9"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="16"/>
+      <c r="A31"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
       <c r="I31"/>
       <c r="J31"/>
       <c r="K31"/>
@@ -2469,14 +2394,14 @@
       <c r="AQ31"/>
     </row>
     <row r="32" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="9"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="16"/>
+      <c r="A32"/>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
       <c r="I32"/>
       <c r="J32"/>
       <c r="K32"/>
@@ -2514,14 +2439,14 @@
       <c r="AQ32"/>
     </row>
     <row r="33" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="9"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="16"/>
+      <c r="A33"/>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
       <c r="I33"/>
       <c r="J33"/>
       <c r="K33"/>
@@ -2559,14 +2484,14 @@
       <c r="AQ33"/>
     </row>
     <row r="34" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="9"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="16"/>
+      <c r="A34"/>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
       <c r="I34"/>
       <c r="J34"/>
       <c r="K34"/>
@@ -2603,15 +2528,15 @@
       <c r="AP34"/>
       <c r="AQ34"/>
     </row>
-    <row r="35" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="10"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="17"/>
-      <c r="D35" s="17"/>
-      <c r="E35" s="17"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="18"/>
+    <row r="35" spans="1:43" s="2" customFormat="1" ht="40" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35"/>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
       <c r="I35"/>
       <c r="J35"/>
       <c r="K35"/>
@@ -2648,15 +2573,15 @@
       <c r="AP35"/>
       <c r="AQ35"/>
     </row>
-    <row r="36" spans="1:43" s="2" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="A36" s="5"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
+    <row r="36" spans="1:43" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A36"/>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
       <c r="I36"/>
       <c r="J36"/>
       <c r="K36"/>
@@ -2721,38 +2646,200 @@
     <row r="62" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="63" customFormat="1" x14ac:dyDescent="0.15"/>
     <row r="64" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="65" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="1"/>
+    </row>
+    <row r="66" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="1"/>
+    </row>
+    <row r="67" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="1"/>
+    </row>
+    <row r="68" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="1"/>
+    </row>
+    <row r="69" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="1"/>
+    </row>
+    <row r="70" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+      <c r="G70" s="1"/>
+      <c r="H70" s="1"/>
+    </row>
+    <row r="71" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+      <c r="G71" s="1"/>
+      <c r="H71" s="1"/>
+    </row>
+    <row r="72" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+      <c r="G72" s="1"/>
+      <c r="H72" s="1"/>
+    </row>
+    <row r="73" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+      <c r="G73" s="1"/>
+      <c r="H73" s="1"/>
+    </row>
+    <row r="74" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+      <c r="G74" s="1"/>
+      <c r="H74" s="1"/>
+    </row>
+    <row r="75" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+      <c r="G75" s="1"/>
+      <c r="H75" s="1"/>
+    </row>
+    <row r="76" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+      <c r="G76" s="1"/>
+      <c r="H76" s="1"/>
+    </row>
+    <row r="77" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+      <c r="G77" s="1"/>
+      <c r="H77" s="1"/>
+    </row>
+    <row r="78" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+      <c r="G78" s="1"/>
+      <c r="H78" s="1"/>
+    </row>
+    <row r="79" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+      <c r="G79" s="1"/>
+      <c r="H79" s="1"/>
+    </row>
+    <row r="80" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+      <c r="G80" s="1"/>
+      <c r="H80" s="1"/>
+    </row>
+    <row r="81" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+      <c r="G81" s="1"/>
+      <c r="H81" s="1"/>
+    </row>
+    <row r="82" spans="1:8" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="A14:H14"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A5:H5"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A3:E3"/>
     <mergeCell ref="A4:E4"/>
     <mergeCell ref="F3:H3"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="A19:H19"/>
-    <mergeCell ref="A28:H28"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A5:H5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>